<commit_message>
Update spreadsheet tab label
</commit_message>
<xml_diff>
--- a/charter-schools/Public-vs-Charter-Comparison-2017.xlsx
+++ b/charter-schools/Public-vs-Charter-Comparison-2017.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Charter Schools" sheetId="1" r:id="rId1"/>
+    <sheet name="Charter Schools in Ohio" sheetId="1" r:id="rId1"/>
     <sheet name="Public Schools in Ohio" sheetId="2" r:id="rId2"/>
     <sheet name="Frequencies" sheetId="3" r:id="rId3"/>
-    <sheet name="%Freq of School Type" sheetId="4" r:id="rId4"/>
+    <sheet name="% Freq of School Type" sheetId="4" r:id="rId4"/>
     <sheet name="% of Each Grade" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -4868,7 +4868,7 @@
   <dimension ref="A1:H277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19205,7 +19205,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="16">
-        <f>COUNTIF('Charter Schools'!C:C, A3)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A3)</f>
         <v>2</v>
       </c>
       <c r="D3" s="16">
@@ -19213,7 +19213,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="16">
-        <f>COUNTIF('Charter Schools'!D:D, A3)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A3)</f>
         <v>6</v>
       </c>
       <c r="F3" s="16">
@@ -19221,7 +19221,7 @@
         <v>129</v>
       </c>
       <c r="G3" s="16">
-        <f>COUNTIF('Charter Schools'!E:E, A3)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A3)</f>
         <v>33</v>
       </c>
       <c r="I3" s="22"/>
@@ -19238,7 +19238,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="16">
-        <f>COUNTIF('Charter Schools'!C:C, A4)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A4)</f>
         <v>4</v>
       </c>
       <c r="D4" s="16">
@@ -19246,7 +19246,7 @@
         <v>111</v>
       </c>
       <c r="E4" s="16">
-        <f>COUNTIF('Charter Schools'!D:D, A4)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A4)</f>
         <v>9</v>
       </c>
       <c r="F4" s="16">
@@ -19254,7 +19254,7 @@
         <v>208</v>
       </c>
       <c r="G4" s="16">
-        <f>COUNTIF('Charter Schools'!E:E, A4)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A4)</f>
         <v>41</v>
       </c>
       <c r="I4" s="22"/>
@@ -19270,7 +19270,7 @@
         <v>214</v>
       </c>
       <c r="C5" s="16">
-        <f>COUNTIF('Charter Schools'!C:C, A5)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A5)</f>
         <v>10</v>
       </c>
       <c r="D5" s="16">
@@ -19278,7 +19278,7 @@
         <v>107</v>
       </c>
       <c r="E5" s="16">
-        <f>COUNTIF('Charter Schools'!D:D, A5)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A5)</f>
         <v>2</v>
       </c>
       <c r="F5" s="16">
@@ -19286,7 +19286,7 @@
         <v>53</v>
       </c>
       <c r="G5" s="16">
-        <f>COUNTIF('Charter Schools'!E:E, A5)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A5)</f>
         <v>53</v>
       </c>
       <c r="I5" s="22"/>
@@ -19302,7 +19302,7 @@
         <v>309</v>
       </c>
       <c r="C6" s="16">
-        <f>COUNTIF('Charter Schools'!C:C, A6)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A6)</f>
         <v>85</v>
       </c>
       <c r="D6" s="16">
@@ -19310,7 +19310,7 @@
         <v>92</v>
       </c>
       <c r="E6" s="16">
-        <f>COUNTIF('Charter Schools'!D:D, A6)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A6)</f>
         <v>9</v>
       </c>
       <c r="F6" s="16">
@@ -19318,7 +19318,7 @@
         <v>153</v>
       </c>
       <c r="G6" s="16">
-        <f>COUNTIF('Charter Schools'!E:E, A6)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A6)</f>
         <v>72</v>
       </c>
       <c r="I6" s="22"/>
@@ -19334,7 +19334,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="16">
-        <f>COUNTIF('Charter Schools'!C:C, A7)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A7)</f>
         <v>165</v>
       </c>
       <c r="D7" s="16">
@@ -19342,7 +19342,7 @@
         <v>293</v>
       </c>
       <c r="E7" s="16">
-        <f>COUNTIF('Charter Schools'!D:D, A7)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A7)</f>
         <v>217</v>
       </c>
       <c r="F7" s="16">
@@ -19350,7 +19350,7 @@
         <v>65</v>
       </c>
       <c r="G7" s="16">
-        <f>COUNTIF('Charter Schools'!E:E, A7)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A7)</f>
         <v>54</v>
       </c>
       <c r="I7" s="22"/>
@@ -19366,7 +19366,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="16">
-        <f>COUNTIF('Charter Schools'!C:C, A8)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A8)</f>
         <v>10</v>
       </c>
       <c r="D8" s="16">
@@ -19374,7 +19374,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="16">
-        <f>COUNTIF('Charter Schools'!D:D, A8)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A8)</f>
         <v>33</v>
       </c>
       <c r="F8" s="16">
@@ -19382,7 +19382,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="16">
-        <f>COUNTIF('Charter Schools'!E:E, A8)</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A8)</f>
         <v>23</v>
       </c>
       <c r="I8" s="22"/>
@@ -19477,7 +19477,7 @@
         <v>2.1381578947368422E-2</v>
       </c>
       <c r="C3" s="15">
-        <f>COUNTIF('Charter Schools'!C:C, A3) / C9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A3) / C9</f>
         <v>7.246376811594203E-3</v>
       </c>
       <c r="D3" s="15">
@@ -19485,7 +19485,7 @@
         <v>8.2236842105263153E-3</v>
       </c>
       <c r="E3" s="15">
-        <f>COUNTIF('Charter Schools'!D:D, A3) / E9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A3) / E9</f>
         <v>2.1739130434782608E-2</v>
       </c>
       <c r="F3" s="15">
@@ -19493,7 +19493,7 @@
         <v>0.21217105263157895</v>
       </c>
       <c r="G3" s="15">
-        <f>COUNTIF('Charter Schools'!E:E, A3) / G9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A3) / G9</f>
         <v>0.11956521739130435</v>
       </c>
     </row>
@@ -19506,7 +19506,7 @@
         <v>8.7171052631578941E-2</v>
       </c>
       <c r="C4" s="15">
-        <f>COUNTIF('Charter Schools'!C:C, A4) / C9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A4) / C9</f>
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="D4" s="15">
@@ -19514,7 +19514,7 @@
         <v>0.18256578947368421</v>
       </c>
       <c r="E4" s="15">
-        <f>COUNTIF('Charter Schools'!D:D, A4) / E9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A4) / E9</f>
         <v>3.2608695652173912E-2</v>
       </c>
       <c r="F4" s="15">
@@ -19522,7 +19522,7 @@
         <v>0.34210526315789475</v>
       </c>
       <c r="G4" s="15">
-        <f>COUNTIF('Charter Schools'!E:E, A4) / G9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A4) / G9</f>
         <v>0.14855072463768115</v>
       </c>
     </row>
@@ -19535,7 +19535,7 @@
         <v>0.35197368421052633</v>
       </c>
       <c r="C5" s="15">
-        <f>COUNTIF('Charter Schools'!C:C, A5) / C9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A5) / C9</f>
         <v>3.6231884057971016E-2</v>
       </c>
       <c r="D5" s="15">
@@ -19543,7 +19543,7 @@
         <v>0.17598684210526316</v>
       </c>
       <c r="E5" s="15">
-        <f>COUNTIF('Charter Schools'!D:D, A5) / E9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A5) / E9</f>
         <v>7.246376811594203E-3</v>
       </c>
       <c r="F5" s="15">
@@ -19551,7 +19551,7 @@
         <v>8.7171052631578941E-2</v>
       </c>
       <c r="G5" s="15">
-        <f>COUNTIF('Charter Schools'!E:E, A5) / G9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A5) / G9</f>
         <v>0.19202898550724637</v>
       </c>
     </row>
@@ -19564,7 +19564,7 @@
         <v>0.50822368421052633</v>
       </c>
       <c r="C6" s="15">
-        <f>COUNTIF('Charter Schools'!C:C, A6) / C9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A6) / C9</f>
         <v>0.3079710144927536</v>
       </c>
       <c r="D6" s="15">
@@ -19572,7 +19572,7 @@
         <v>0.15131578947368421</v>
       </c>
       <c r="E6" s="15">
-        <f>COUNTIF('Charter Schools'!D:D, A6) / E9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A6) / E9</f>
         <v>3.2608695652173912E-2</v>
       </c>
       <c r="F6" s="15">
@@ -19580,7 +19580,7 @@
         <v>0.25164473684210525</v>
       </c>
       <c r="G6" s="15">
-        <f>COUNTIF('Charter Schools'!E:E, A6) / G9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A6) / G9</f>
         <v>0.2608695652173913</v>
       </c>
     </row>
@@ -19593,7 +19593,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="C7" s="15">
-        <f>COUNTIF('Charter Schools'!C:C, A7) / C9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A7) / C9</f>
         <v>0.59782608695652173</v>
       </c>
       <c r="D7" s="15">
@@ -19601,7 +19601,7 @@
         <v>0.48190789473684209</v>
       </c>
       <c r="E7" s="15">
-        <f>COUNTIF('Charter Schools'!D:D, A7) / E9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A7) / E9</f>
         <v>0.78623188405797106</v>
       </c>
       <c r="F7" s="15">
@@ -19609,7 +19609,7 @@
         <v>0.1069078947368421</v>
       </c>
       <c r="G7" s="15">
-        <f>COUNTIF('Charter Schools'!E:E, A7) / G9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A7) / G9</f>
         <v>0.19565217391304349</v>
       </c>
     </row>
@@ -19622,7 +19622,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="15">
-        <f>COUNTIF('Charter Schools'!C:C, A8) / C9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A8) / C9</f>
         <v>3.6231884057971016E-2</v>
       </c>
       <c r="D8" s="15">
@@ -19630,7 +19630,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="15">
-        <f>COUNTIF('Charter Schools'!D:D, A8) / E9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A8) / E9</f>
         <v>0.11956521739130435</v>
       </c>
       <c r="F8" s="15">
@@ -19638,7 +19638,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="15">
-        <f>COUNTIF('Charter Schools'!E:E, A8) / G9</f>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A8) / G9</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -19679,7 +19679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the data to exclude schools not rated from percentages
</commit_message>
<xml_diff>
--- a/charter-schools/Public-vs-Charter-Comparison-2017.xlsx
+++ b/charter-schools/Public-vs-Charter-Comparison-2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Charter Schools in Ohio" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3885" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3884" uniqueCount="1109">
   <si>
     <t>A+ Arts Academy</t>
   </si>
@@ -3355,6 +3355,21 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Charter totals do not include the ten NR grades.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3365,7 +3380,14 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3431,15 +3453,15 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3452,36 +3474,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3489,22 +3511,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3562,7 +3584,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Grades Earned</a:t>
+              <a:t> Grades Earned by Schools in 2017</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3633,9 +3655,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'% of Each Grade'!$A$3:$A$8</c:f>
+              <c:f>'% of Each Grade'!$A$3:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -3651,18 +3673,15 @@
                 <c:pt idx="4">
                   <c:v>F</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>NR</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'% of Each Grade'!$B$3:$B$8</c:f>
+              <c:f>'% of Each Grade'!$B$3:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.866666666666667</c:v>
                 </c:pt>
@@ -3677,9 +3696,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.103260869565217</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3714,9 +3730,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'% of Each Grade'!$A$3:$A$8</c:f>
+              <c:f>'% of Each Grade'!$A$3:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -3732,18 +3748,15 @@
                 <c:pt idx="4">
                   <c:v>F</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>NR</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'% of Each Grade'!$C$3:$C$8</c:f>
+              <c:f>'% of Each Grade'!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.133333333333333</c:v>
                 </c:pt>
@@ -3758,9 +3771,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.896739130434783</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4573,13 +4583,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4867,7 +4877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -19144,7 +19154,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19397,19 +19407,22 @@
         <v>608</v>
       </c>
       <c r="C9" s="24">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D9" s="24">
         <v>608</v>
       </c>
       <c r="E9" s="24">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="F9" s="24">
         <v>608</v>
       </c>
       <c r="G9" s="24">
-        <v>276</v>
+        <v>266</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>1108</v>
       </c>
     </row>
   </sheetData>
@@ -19424,10 +19437,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19473,28 +19486,28 @@
         <v>53</v>
       </c>
       <c r="B3" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!B:B, A3) / B9</f>
+        <f>COUNTIF('Public Schools in Ohio'!B:B, A3) / B8</f>
         <v>2.1381578947368422E-2</v>
       </c>
       <c r="C3" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!C:C, A3) / C9</f>
-        <v>7.246376811594203E-3</v>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A3) / C8</f>
+        <v>7.5187969924812026E-3</v>
       </c>
       <c r="D3" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!C:C, A3) / D9</f>
+        <f>COUNTIF('Public Schools in Ohio'!C:C, A3) / D8</f>
         <v>8.2236842105263153E-3</v>
       </c>
       <c r="E3" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!D:D, A3) / E9</f>
-        <v>2.1739130434782608E-2</v>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A3) / E8</f>
+        <v>2.2556390977443608E-2</v>
       </c>
       <c r="F3" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!D:D, A3) / F9</f>
+        <f>COUNTIF('Public Schools in Ohio'!D:D, A3) / F8</f>
         <v>0.21217105263157895</v>
       </c>
       <c r="G3" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!E:E, A3) / G9</f>
-        <v>0.11956521739130435</v>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A3) / G8</f>
+        <v>0.12406015037593984</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -19502,28 +19515,28 @@
         <v>21</v>
       </c>
       <c r="B4" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!B:B, A4) / B9</f>
+        <f>COUNTIF('Public Schools in Ohio'!B:B, A4) / B8</f>
         <v>8.7171052631578941E-2</v>
       </c>
       <c r="C4" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!C:C, A4) / C9</f>
-        <v>1.4492753623188406E-2</v>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A4) / C8</f>
+        <v>1.5037593984962405E-2</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!C:C, A4) / D9</f>
+        <f>COUNTIF('Public Schools in Ohio'!C:C, A4) / D8</f>
         <v>0.18256578947368421</v>
       </c>
       <c r="E4" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!D:D, A4) / E9</f>
-        <v>3.2608695652173912E-2</v>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A4) / E8</f>
+        <v>3.3834586466165412E-2</v>
       </c>
       <c r="F4" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!D:D, A4) / F9</f>
+        <f>COUNTIF('Public Schools in Ohio'!D:D, A4) / F8</f>
         <v>0.34210526315789475</v>
       </c>
       <c r="G4" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!E:E, A4) / G9</f>
-        <v>0.14855072463768115</v>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A4) / G8</f>
+        <v>0.15413533834586465</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -19531,28 +19544,28 @@
         <v>38</v>
       </c>
       <c r="B5" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!B:B, A5) / B9</f>
+        <f>COUNTIF('Public Schools in Ohio'!B:B, A5) / B8</f>
         <v>0.35197368421052633</v>
       </c>
       <c r="C5" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!C:C, A5) / C9</f>
-        <v>3.6231884057971016E-2</v>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A5) / C8</f>
+        <v>3.7593984962406013E-2</v>
       </c>
       <c r="D5" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!C:C, A5) / D9</f>
+        <f>COUNTIF('Public Schools in Ohio'!C:C, A5) / D8</f>
         <v>0.17598684210526316</v>
       </c>
       <c r="E5" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!D:D, A5) / E9</f>
-        <v>7.246376811594203E-3</v>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A5) / E8</f>
+        <v>7.5187969924812026E-3</v>
       </c>
       <c r="F5" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!D:D, A5) / F9</f>
+        <f>COUNTIF('Public Schools in Ohio'!D:D, A5) / F8</f>
         <v>8.7171052631578941E-2</v>
       </c>
       <c r="G5" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!E:E, A5) / G9</f>
-        <v>0.19202898550724637</v>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A5) / G8</f>
+        <v>0.19924812030075187</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -19560,28 +19573,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!B:B, A6) / B9</f>
+        <f>COUNTIF('Public Schools in Ohio'!B:B, A6) / B8</f>
         <v>0.50822368421052633</v>
       </c>
       <c r="C6" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!C:C, A6) / C9</f>
-        <v>0.3079710144927536</v>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A6) / C8</f>
+        <v>0.31954887218045114</v>
       </c>
       <c r="D6" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!C:C, A6) / D9</f>
+        <f>COUNTIF('Public Schools in Ohio'!C:C, A6) / D8</f>
         <v>0.15131578947368421</v>
       </c>
       <c r="E6" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!D:D, A6) / E9</f>
-        <v>3.2608695652173912E-2</v>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A6) / E8</f>
+        <v>3.3834586466165412E-2</v>
       </c>
       <c r="F6" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!D:D, A6) / F9</f>
+        <f>COUNTIF('Public Schools in Ohio'!D:D, A6) / F8</f>
         <v>0.25164473684210525</v>
       </c>
       <c r="G6" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!E:E, A6) / G9</f>
-        <v>0.2608695652173913</v>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A6) / G8</f>
+        <v>0.27067669172932329</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -19589,80 +19602,51 @@
         <v>2</v>
       </c>
       <c r="B7" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!B:B, A7) / B9</f>
+        <f>COUNTIF('Public Schools in Ohio'!B:B, A7) / B8</f>
         <v>3.125E-2</v>
       </c>
       <c r="C7" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!C:C, A7) / C9</f>
-        <v>0.59782608695652173</v>
+        <f>COUNTIF('Charter Schools in Ohio'!C:C, A7) / C8</f>
+        <v>0.62030075187969924</v>
       </c>
       <c r="D7" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!C:C, A7)  / D9</f>
+        <f>COUNTIF('Public Schools in Ohio'!C:C, A7)  / D8</f>
         <v>0.48190789473684209</v>
       </c>
       <c r="E7" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!D:D, A7) / E9</f>
-        <v>0.78623188405797106</v>
+        <f>COUNTIF('Charter Schools in Ohio'!D:D, A7) / E8</f>
+        <v>0.81578947368421051</v>
       </c>
       <c r="F7" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!D:D, A7) / F9</f>
+        <f>COUNTIF('Public Schools in Ohio'!D:D, A7) / F8</f>
         <v>0.1069078947368421</v>
       </c>
       <c r="G7" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!E:E, A7) / G9</f>
-        <v>0.19565217391304349</v>
+        <f>COUNTIF('Charter Schools in Ohio'!E:E, A7) / G8</f>
+        <v>0.20300751879699247</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!B:B, A8) / B9</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!C:C, A8) / C9</f>
-        <v>3.6231884057971016E-2</v>
-      </c>
-      <c r="D8" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!C:C, A8) / D9</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!D:D, A8) / E9</f>
-        <v>0.11956521739130435</v>
-      </c>
-      <c r="F8" s="15">
-        <f>COUNTIF('Public Schools in Ohio'!D:D, A8) / F9</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="15">
-        <f>COUNTIF('Charter Schools in Ohio'!E:E, A8) / G9</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A8" s="14" t="s">
         <v>1107</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B8" s="11">
         <v>608</v>
       </c>
-      <c r="C9" s="11">
-        <v>276</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C8" s="11">
+        <v>266</v>
+      </c>
+      <c r="D8" s="11">
         <v>608</v>
       </c>
-      <c r="E9" s="11">
-        <v>276</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="E8" s="11">
+        <v>266</v>
+      </c>
+      <c r="F8" s="11">
         <v>608</v>
       </c>
-      <c r="G9" s="11">
-        <v>276</v>
+      <c r="G8" s="11">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -19677,10 +19661,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19870,35 +19854,6 @@
         <v>0.45378151260504201</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="25">
-        <f>Frequencies!B8 / SUM(Frequencies!B8,Frequencies!C8)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="25">
-        <f>Frequencies!C8 / SUM(Frequencies!B8,Frequencies!C8)</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="25">
-        <f>Frequencies!D8 / SUM(Frequencies!D8,Frequencies!E8)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="25">
-        <f>Frequencies!E8 / SUM(Frequencies!D8,Frequencies!E8)</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="25">
-        <f>Frequencies!F8 / SUM(Frequencies!F8,Frequencies!G8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="25">
-        <f>Frequencies!G8 / SUM(Frequencies!F8,Frequencies!G8)</f>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>

</xml_diff>